<commit_message>
made all the stable isos fumed values 2018 and 2019
</commit_message>
<xml_diff>
--- a/data/flux/flux_orders.xlsx
+++ b/data/flux/flux_orders.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="144">
   <si>
     <t xml:space="preserve">sample id</t>
   </si>
@@ -303,6 +303,156 @@
   </si>
   <si>
     <t xml:space="preserve">4-45_843m_nw4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-58_170m_NO2_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-58_170m_NO2_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-58_570m_NO2_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1_58_570m_NO2_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-58_570m_NO2_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-58_370m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-58_370m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-58_370m_NO2_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-58_102m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-58_102m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-58_102m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-58_770m_net_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-58_770m_net_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-58_770m_net_nw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-59_130m_NO2_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-59_130m_NO2_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-59_130m_NO2_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-59_300m_Fe_top_split</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-59_700m_NO2_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-59_700m_NO2_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-59_700m_NO2_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-59_965m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-59_965m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-59_965m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-52_173m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-52_173m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-52_173m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-52_965m_top/+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-54_402m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-54_402m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-54_171m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-54_200m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-54_200m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-50_100m_NO2_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-50_300m_NO2_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-50_300m_NO2_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-50_100m_NO2_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-50_100m_NO2_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-50_300m_NO2_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-55_490m_top/+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-55_390m_top_Clint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-55_90m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-55_490m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-55_90m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-51_520m_NO2_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-51_520m_NO2_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-53_278m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-53_107m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-53_107m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-53_107m_ctl</t>
   </si>
 </sst>
 </file>
@@ -312,7 +462,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -332,6 +482,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -376,8 +532,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -905,14 +1065,270 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>